<commit_message>
[UPDATE]: actualización con información en drive
</commit_message>
<xml_diff>
--- a/docs/textArticle.xlsx
+++ b/docs/textArticle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff2dc98e2a8f9132/University Proyect/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{7DC7D18E-251B-4AEF-96CE-E4F5582B8889}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{E4923A8C-9537-4252-A189-21C7EE621F9F}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="8_{7DC7D18E-251B-4AEF-96CE-E4F5582B8889}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{B592493F-7676-4A14-9DC4-76C7A4973797}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19545" windowHeight="8385" xr2:uid="{C6E18974-3E46-4541-A374-4EC13FC6C075}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Según lo estudiado en el artículo Design Principles and Top Non-Fullerene Acceptor Candidates for Organic Photovoltaics, vemos que se sigue la siguiente secuencia en la ejecución que lleva a las móleculas deseadas:</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>¿La razón por la cual se crean conformers en un inicio, es para dar diferentes configuraciones desde las cuales al aplicar el MMFF se logre una mayor probabilidad de encontrar el mínimo global de la energía?</t>
-  </si>
-  <si>
-    <t>Cómo utilizarón la reducción de moleculas a través de obfit? Este método alínea la moleculas y elimina aquellas que son iguales, o qué se considera?</t>
   </si>
 </sst>
 </file>
@@ -512,7 +509,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,9 +559,6 @@
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="4" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">

</xml_diff>

<commit_message>
agregado gitignore y agregado datos a textArticle
</commit_message>
<xml_diff>
--- a/docs/textArticle.xlsx
+++ b/docs/textArticle.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff2dc98e2a8f9132/University Proyect/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{7DC7D18E-251B-4AEF-96CE-E4F5582B8889}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{B592493F-7676-4A14-9DC4-76C7A4973797}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{7DC7D18E-251B-4AEF-96CE-E4F5582B8889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{83DF9397-C8CB-4A22-B5D8-3462B95DCB53}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19545" windowHeight="8385" xr2:uid="{C6E18974-3E46-4541-A374-4EC13FC6C075}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{C6E18974-3E46-4541-A374-4EC13FC6C075}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Según lo estudiado en el artículo Design Principles and Top Non-Fullerene Acceptor Candidates for Organic Photovoltaics, vemos que se sigue la siguiente secuencia en la ejecución que lleva a las móleculas deseadas:</t>
   </si>
@@ -110,12 +104,29 @@
   <si>
     <t>¿La razón por la cual se crean conformers en un inicio, es para dar diferentes configuraciones desde las cuales al aplicar el MMFF se logre una mayor probabilidad de encontrar el mínimo global de la energía?</t>
   </si>
+  <si>
+    <t>Las células solares orgánicas nos muestran un camino interesante hacia el uso de energías renovables ecológicas y amigables. Eso nos ayudará a mitigar el efecto o huella de carbono. Se están cuestionando formas eficientes de convertir la energía solar en electricidad, como el uso de materiales, buscando las mejores propiedades que permitan una óptima conversión energética. Este trabajo explora el uso de técnicas de aprendizaje automático (ML) para ayudar a optimizar propiedades moleculares como el orbital molecular de alta ocupación (HOMO) y las energías de orbital molecular desocupado más bajo (LUMO), así como el cálculo y calibración de la eficiencia de conversión de potencia (PCE). ) con el ánimo de buscar grandes candidatas a moléculas orgánicas para su uso como sistemas donante-receptor en células solares. En particular, probamos una calibración del proceso gaussiano como un modelo ML en un conjunto de moléculas reportadas en la literatura [1] y discutimos algunos aspectos tanto de las propiedades químicas como de la ventaja de usar ML</t>
+  </si>
+  <si>
+    <r>
+      <t>Keywords:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Organic Solar Cell, Small Molecules, Machine Learning, Computational Chemistry, Quantum Systems.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +140,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -172,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -192,6 +217,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,7 +238,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -508,11 +536,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123720D3-AFD9-4B01-AE0E-0EAED385E34E}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="91.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" style="1" customWidth="1"/>
@@ -560,7 +588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -589,15 +617,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:4" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" s="3"/>
       <c r="C8" s="2" t="s">
         <v>11</v>

</xml_diff>